<commit_message>
Commit check point 1
</commit_message>
<xml_diff>
--- a/Data_Karyawan.xlsx
+++ b/Data_Karyawan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FAISHAL\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FAISHAL\Documents\payroll_inix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48E173A5-00D4-457F-8B29-5530464EA46C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA2F3446-7A0A-4419-9159-2E626FE2A5EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="81">
   <si>
     <t>No.Urut</t>
   </si>
@@ -79,9 +79,6 @@
     <t>TK/0</t>
   </si>
   <si>
-    <t>faishalfh1@gmail.com</t>
-  </si>
-  <si>
     <t>ACHMAD FAISOL</t>
   </si>
   <si>
@@ -148,69 +145,9 @@
     <t>DWI RAMA SURYA MUSTIKA</t>
   </si>
   <si>
-    <t>faisol@inixindo.id</t>
-  </si>
-  <si>
-    <t>didiksby9@gmail.com</t>
-  </si>
-  <si>
-    <t>ellysjuliati@gmail.com</t>
-  </si>
-  <si>
-    <t>satuhar72@gmail.com</t>
-  </si>
-  <si>
-    <t>mutiahindriastuti@gmail.com</t>
-  </si>
-  <si>
-    <t>denny.willyanto@gmail.com</t>
-  </si>
-  <si>
-    <t>drv.inixindosurabaya@gmail.com</t>
-  </si>
-  <si>
-    <t>wildaaziatulqolbi@gmail.com</t>
-  </si>
-  <si>
-    <t>deayulis@gmail.com</t>
-  </si>
-  <si>
-    <t>rionandha19@gmail.com</t>
-  </si>
-  <si>
-    <t>anovredo@gmail.com</t>
-  </si>
-  <si>
-    <t>evan.design003@gmail.com</t>
-  </si>
-  <si>
-    <t>devafeli7@gmail.com</t>
-  </si>
-  <si>
-    <t>aku.hayyu@gmail.com</t>
-  </si>
-  <si>
-    <t>faradinayovita36@gmail.com</t>
-  </si>
-  <si>
-    <t>priscilayunita14@gmail.com</t>
-  </si>
-  <si>
-    <t>fandimalang41@gmail.com</t>
-  </si>
-  <si>
-    <t>triaanandarhy@gmail.com</t>
-  </si>
-  <si>
     <t>saptowahyusudrajat@gmail.com</t>
   </si>
   <si>
-    <t>echacame@gmail.com</t>
-  </si>
-  <si>
-    <t>dwiramasm@gmail.com</t>
-  </si>
-  <si>
     <t>INSTRUKTUR</t>
   </si>
   <si>
@@ -251,15 +188,87 @@
   </si>
   <si>
     <t>ACCOUNT EXECUTIVE</t>
+  </si>
+  <si>
+    <t>faishalfh1.work@gmail.com</t>
+  </si>
+  <si>
+    <t>karyawan1@perusahaan.com</t>
+  </si>
+  <si>
+    <t>karyawan2@perusahaan.com</t>
+  </si>
+  <si>
+    <t>karyawan3@perusahaan.com</t>
+  </si>
+  <si>
+    <t>karyawan4@perusahaan.com</t>
+  </si>
+  <si>
+    <t>karyawan5@perusahaan.com</t>
+  </si>
+  <si>
+    <t>karyawan6@perusahaan.com</t>
+  </si>
+  <si>
+    <t>karyawan7@perusahaan.com</t>
+  </si>
+  <si>
+    <t>karyawan8@perusahaan.com</t>
+  </si>
+  <si>
+    <t>karyawan9@perusahaan.com</t>
+  </si>
+  <si>
+    <t>karyawan10@perusahaan.com</t>
+  </si>
+  <si>
+    <t>karyawan11@perusahaan.com</t>
+  </si>
+  <si>
+    <t>karyawan12@perusahaan.com</t>
+  </si>
+  <si>
+    <t>karyawan13@perusahaan.com</t>
+  </si>
+  <si>
+    <t>karyawan14@perusahaan.com</t>
+  </si>
+  <si>
+    <t>karyawan15@perusahaan.com</t>
+  </si>
+  <si>
+    <t>karyawan16@perusahaan.com</t>
+  </si>
+  <si>
+    <t>karyawan17@perusahaan.com</t>
+  </si>
+  <si>
+    <t>karyawan18@perusahaan.com</t>
+  </si>
+  <si>
+    <t>karyawan19@perusahaan.com</t>
+  </si>
+  <si>
+    <t>karyawan20@perusahaan.com</t>
+  </si>
+  <si>
+    <t>0002</t>
+  </si>
+  <si>
+    <t>0003</t>
+  </si>
+  <si>
+    <t>1003010y6.15</t>
+  </si>
+  <si>
+    <t>1038U207.85</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0000"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -312,22 +321,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -636,29 +641,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.6640625" customWidth="1"/>
-    <col min="4" max="4" width="17.77734375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="30.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -705,27 +710,27 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="5">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="D2" s="4">
         <v>9901</v>
       </c>
       <c r="E2" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="F2" t="s">
         <v>15</v>
       </c>
-      <c r="G2">
-        <v>10030106.15</v>
+      <c r="G2" t="s">
+        <v>79</v>
       </c>
       <c r="H2">
         <v>1038207.85</v>
@@ -752,21 +757,21 @@
         <v>1533913</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="5">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D3" s="6">
-        <v>2</v>
-      </c>
-      <c r="E3" s="2" t="s">
         <v>43</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" t="s">
+        <v>58</v>
       </c>
       <c r="F3" t="s">
         <v>16</v>
@@ -799,21 +804,21 @@
         <v>892302</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="5">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D4" s="6">
-        <v>3</v>
+        <v>43</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="E4" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="F4" t="s">
         <v>17</v>
@@ -846,21 +851,21 @@
         <v>1364955</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="5">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="D5" s="4">
         <v>1303</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="F5" t="s">
         <v>18</v>
@@ -893,21 +898,21 @@
         <v>1019127</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="D6" s="4">
         <v>1302</v>
       </c>
       <c r="E6" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="F6" t="s">
         <v>15</v>
@@ -940,21 +945,21 @@
         <v>849304</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="5">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="D7" s="4">
         <v>1301</v>
       </c>
       <c r="E7" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="F7" t="s">
         <v>18</v>
@@ -987,21 +992,21 @@
         <v>453589</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="5">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="D8" s="4">
         <v>1501</v>
       </c>
       <c r="E8" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="F8" t="s">
         <v>16</v>
@@ -1034,21 +1039,21 @@
         <v>1442956</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="5">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="D9" s="4">
         <v>1703</v>
       </c>
       <c r="E9" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="F9" t="s">
         <v>17</v>
@@ -1081,21 +1086,21 @@
         <v>543007</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="5">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="D10" s="4">
         <v>1702</v>
       </c>
       <c r="E10" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="F10" t="s">
         <v>16</v>
@@ -1128,21 +1133,21 @@
         <v>1412480</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="5">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="D11" s="4">
         <v>1701</v>
       </c>
       <c r="E11" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="F11" t="s">
         <v>17</v>
@@ -1175,21 +1180,21 @@
         <v>1689225</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="5">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="D12" s="4">
         <v>2001</v>
       </c>
       <c r="E12" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="F12" t="s">
         <v>15</v>
@@ -1197,8 +1202,8 @@
       <c r="G12">
         <v>10030106.15</v>
       </c>
-      <c r="H12">
-        <v>1038207.85</v>
+      <c r="H12" t="s">
+        <v>80</v>
       </c>
       <c r="I12">
         <v>9.3800000000000008</v>
@@ -1222,21 +1227,21 @@
         <v>1533913</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="5">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C13" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="D13" s="4">
         <v>2101</v>
       </c>
       <c r="E13" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="F13" t="s">
         <v>16</v>
@@ -1269,21 +1274,21 @@
         <v>892302</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="5">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C14" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="D14" s="4">
         <v>2201</v>
       </c>
       <c r="E14" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="F14" t="s">
         <v>17</v>
@@ -1316,21 +1321,21 @@
         <v>1364955</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="5">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="D15" s="4">
         <v>2102</v>
       </c>
       <c r="E15" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="F15" t="s">
         <v>18</v>
@@ -1363,21 +1368,21 @@
         <v>1019127</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="5">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C16" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="D16" s="4">
         <v>2301</v>
       </c>
       <c r="E16" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="F16" t="s">
         <v>15</v>
@@ -1410,21 +1415,21 @@
         <v>849304</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A17" s="5">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C17" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="D17" s="4">
         <v>2402</v>
       </c>
       <c r="E17" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="F17" t="s">
         <v>18</v>
@@ -1457,21 +1462,21 @@
         <v>453589</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A18" s="5">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C18" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="D18" s="4">
         <v>2401</v>
       </c>
       <c r="E18" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="F18" t="s">
         <v>16</v>
@@ -1504,21 +1509,21 @@
         <v>1442956</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A19" s="5">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C19" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="D19" s="4">
         <v>2501</v>
       </c>
       <c r="E19" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="F19" t="s">
         <v>17</v>
@@ -1551,21 +1556,21 @@
         <v>543007</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A20" s="5">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C20" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="D20" s="4">
         <v>2502</v>
       </c>
       <c r="E20" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="F20" t="s">
         <v>16</v>
@@ -1598,21 +1603,21 @@
         <v>1412480</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A21" s="5">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C21" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="D21" s="4">
         <v>2504</v>
       </c>
       <c r="E21" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="F21" t="s">
         <v>17</v>
@@ -1645,21 +1650,21 @@
         <v>1689225</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A22" s="5">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C22" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="D22" s="4">
         <v>2505</v>
       </c>
       <c r="E22" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="F22" t="s">
         <v>16</v>
@@ -1692,21 +1697,21 @@
         <v>1412480</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A23" s="5">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C23" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="D23" s="4">
         <v>2506</v>
       </c>
       <c r="E23" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="F23" t="s">
         <v>17</v>
@@ -1741,5 +1746,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="D3:D4" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>